<commit_message>
feat: aumentando o limite do json bodyparser
</commit_message>
<xml_diff>
--- a/filmes.xlsx
+++ b/filmes.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E191"/>
+  <dimension ref="A1:E321"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -568,6 +568,9 @@
       <c r="D10">
         <v>8.8</v>
       </c>
+      <c r="E10" t="str">
+        <v>Um impostor se junta com dois homens para encontrar fortuna num remoto cemitério.</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -582,6 +585,9 @@
       <c r="D11">
         <v>8.8</v>
       </c>
+      <c r="E11" t="str">
+        <v>Os governos dos presidentes Kennedy e Johnson, os eventos do Vietnã e Watergate e outras histórias são mostradas através da perspectiva de um homem do Alabama com baixo quociente intelectual.</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -596,6 +602,9 @@
       <c r="D12">
         <v>8.8</v>
       </c>
+      <c r="E12" t="str">
+        <v>Enquanto Frodo e Sam estão perto de Mordor com a ajuda de Gollum, a divida comunhão luta contra Saruman e os Isengards.</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -610,6 +619,9 @@
       <c r="D13">
         <v>8.8</v>
       </c>
+      <c r="E13" t="str">
+        <v>Um trabalhador de escritório e um fabricante de sabonetes formam um clube de luta clandestino que evolui para algo muito maior.</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -624,6 +636,9 @@
       <c r="D14">
         <v>8.8</v>
       </c>
+      <c r="E14" t="str">
+        <v>Um ladrão que rouba segredos corporativos através da tecnologia de entrar no subconsciente recebe a tarefa inversa de plantar uma idéia na mente do diretor de uma grande empresa.</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -638,6 +653,9 @@
       <c r="D15">
         <v>8.7</v>
       </c>
+      <c r="E15" t="str">
+        <v>Um hacker aprende com os misteriosos rebeldes sobre a verdadeira natureza de sua realidade e seu papel na guerra contra seus controladores.</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -652,6 +670,9 @@
       <c r="D16">
         <v>8.7</v>
       </c>
+      <c r="E16" t="str">
+        <v>A historia do Henry Hill e sua vida na máfia, sua relação com sua esposa Karen Hill e seus colegas da máfia Jimmy Conway e Tommy DeVito no sindicato italo-americano do crime.</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -666,6 +687,9 @@
       <c r="D17">
         <v>8.7</v>
       </c>
+      <c r="E17" t="str">
+        <v>Uma equipe de exploradores viaja através de um buraco de minhoca no espaço, na tentativa de garantir a sobrevivência da humanidade.</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -680,6 +704,9 @@
       <c r="D18">
         <v>8.7</v>
       </c>
+      <c r="E18" t="str">
+        <v>Um criminoso alega insanidade para ser enviado a um centro de saúde mental, onde se rebela contra a opressiva enfermeira e mobiliza os pacientes a quem ela atemoriza.</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -694,6 +721,9 @@
       <c r="D19">
         <v>8.6</v>
       </c>
+      <c r="E19" t="str">
+        <v>Dois detetives, um novato e um veterano, perseguem um assassino em série que usa os sete pecados capitais como motivos.</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -708,6 +738,9 @@
       <c r="D20">
         <v>8.6</v>
       </c>
+      <c r="E20" t="str">
+        <v>Uma jovem deve receber a ajuda de um assassino canibal manipulador e preso para ajudar a capturar outro assassino em série, um louco que ataca suas vítimas.</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -722,6 +755,9 @@
       <c r="D21">
         <v>8.6</v>
       </c>
+      <c r="E21" t="str">
+        <v>Uma aldeia pobre sob a ameaça de bandidos recruta sete samurais para ajudá-los a se defenderem.</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -736,6 +772,9 @@
       <c r="D22">
         <v>8.6</v>
       </c>
+      <c r="E22" t="str">
+        <v>Depois de chegar a Normandía, um grupo de soldados precisa encontrar o único irmão vivo de três que morreram na guerra.</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -750,6 +789,9 @@
       <c r="D23">
         <v>8.6</v>
       </c>
+      <c r="E23" t="str">
+        <v>As vidas dos guardas de corredor da morte são afetadas por um dos detidos: um homem afro-americano acusado pelo assassinato e estupro de uma criança, mas com um presente misterioso.</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -764,6 +806,9 @@
       <c r="D24">
         <v>8.6</v>
       </c>
+      <c r="E24" t="str">
+        <v>Os caminhos de duas crianças divergem nas favelas do Rio, enquanto um se esforça para se tornar um fotógrafo e o outro um chefe do tráfico.</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -778,6 +823,9 @@
       <c r="D25">
         <v>8.6</v>
       </c>
+      <c r="E25" t="str">
+        <v>Um ciborgue, idêntico ao que falhou em matar Sarah Connor, agora deve proteger o filho de dez anos dela, John, de um ciborgue ainda mais avançado e poderoso.</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -792,6 +840,9 @@
       <c r="D26">
         <v>8.6</v>
       </c>
+      <c r="E26" t="str">
+        <v>Luke Skywalker une forças com um cavaleiro Jedi, um piloto arrogante, um Wookiee e dois andróides para salvar a galáxia da estação de batalha destruidora do Império, enquanto tenta resgatar a Princesa Leia do misterioso Darth Vader.</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -806,6 +857,9 @@
       <c r="D27">
         <v>8.5</v>
       </c>
+      <c r="E27" t="str">
+        <v>Um musico judeu luta para sobreviver a destruição de Varsóvia durante a segunda guerra mundial.</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -820,6 +874,9 @@
       <c r="D28">
         <v>8.5</v>
       </c>
+      <c r="E28" t="str">
+        <v>Um general romano planeja a melhor vingança contra o imperador corrupto que matou sua familia e o fez escravo.</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -834,6 +891,9 @@
       <c r="D29">
         <v>8.5</v>
       </c>
+      <c r="E29" t="str">
+        <v>Desempregados, a família de Ki-taek (Song Kang-ho) nutre um interesse peculiar pela família Park até que eles se veem presos em um inesperado incidente.</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -848,6 +908,9 @@
       <c r="D30">
         <v>8.5</v>
       </c>
+      <c r="E30" t="str">
+        <v>Uma secretária de Phoenix desvia dinheiro de um cliente de sua empresa, foge e vai a um motel remoto gerido por um jovem sob o domínio da mãe.</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -862,6 +925,9 @@
       <c r="D31">
         <v>8.5</v>
       </c>
+      <c r="E31" t="str">
+        <v>Um menino e sua irmã tentam sobreviver no Japão durante a Segunda Guerra Mundial.</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -876,6 +942,9 @@
       <c r="D32">
         <v>8.5</v>
       </c>
+      <c r="E32" t="str">
+        <v>Um policial disfarçado e um espião estão tentando se identificar enquanto se infiltram em uma gangue irlandesa no sul de Boston.</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -890,6 +959,9 @@
       <c r="D33">
         <v>8.5</v>
       </c>
+      <c r="E33" t="str">
+        <v>Um jovem e promissor baterista se matricula em um conservatório de música onde seus sonhos são guiados por um instrutor que não pára por nada para perceber o potencial de um aluno.</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -904,6 +976,9 @@
       <c r="D34">
         <v>8.6</v>
       </c>
+      <c r="E34" t="str">
+        <v>Um velho samurai ronin chega à casa de um senhor feudal e pede um lugar honroso para cometer suicídio. Mas quando o ronin pede um samurai mais jovem que chegou antes, os eventos seguem um curso inesperado.</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -918,6 +993,9 @@
       <c r="D35">
         <v>8.5</v>
       </c>
+      <c r="E35" t="str">
+        <v>Depois de um trágico acidente, dois magos do palco se engajam em uma batalha para criar a ilusão final enquanto sacrificam tudo o que têm para enganar um ao outro.</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -932,6 +1010,9 @@
       <c r="D36">
         <v>8.5</v>
       </c>
+      <c r="E36" t="str">
+        <v>Um neonazista tenta evitar que seu irmão mais novo tome o mesmo caminho errado que ele.</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -946,6 +1027,9 @@
       <c r="D37">
         <v>8.5</v>
       </c>
+      <c r="E37" t="str">
+        <v>Mathilda, uma menina de 12 anos é levada por Léon, um assassino profissional, depois que sua família é assassinada. Léon e Mathilda formam uma relação incomum, desde que ela se torna sua protegida.</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -960,6 +1044,9 @@
       <c r="D38">
         <v>8.5</v>
       </c>
+      <c r="E38" t="str">
+        <v>Viajando pelo multiverso, Miles Morales conhece um novo time de Pessoas-Aranha, formado por heróis de diversas dimensões. Mas quando os heróis entram em conflito sobre como lidar com uma nova ameaça, Miles se vê em um impasse.</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -974,6 +1061,9 @@
       <c r="D39">
         <v>8.5</v>
       </c>
+      <c r="E39" t="str">
+        <v>Um diretor de cinema lembra como, em sua infância, ele se apaixonou pelo cinema de sua cidade e iniciou uma profunda amizade com o projecionista.</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -988,6 +1078,9 @@
       <c r="D40">
         <v>8.5</v>
       </c>
+      <c r="E40" t="str">
+        <v>Depois de ficar tetraplégico num acidente, um aristocrata contrata um jovem de um bairro pobre para cuidar dele.</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1002,6 +1095,9 @@
       <c r="D41">
         <v>8.5</v>
       </c>
+      <c r="E41" t="str">
+        <v>O único sobrevivente conta os torcidos eventos duma luta com pistolas num bote, quanfo cinco criminais eram levados pela polícia.</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1016,6 +1112,9 @@
       <c r="D42">
         <v>8.5</v>
       </c>
+      <c r="E42" t="str">
+        <v>Depois de investigar uma transmissão misteriosa de origem desconhecida, a tripulação de uma nave espacial comercial encontra uma forma de vida mortal.</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1030,6 +1129,9 @@
       <c r="D43">
         <v>8.5</v>
       </c>
+      <c r="E43" t="str">
+        <v>Um fotógrafo em uma cadeira de rodas espiona seus vizinhos pela janela de seu apartamento e está convencido de que um deles cometeu um assassinato.</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1044,6 +1146,9 @@
       <c r="D44">
         <v>8.5</v>
       </c>
+      <c r="E44" t="str">
+        <v>Com a ajuda de um caçador de recompensas alemão, um escravo libertado sai para resgatar sua esposa de um brutal dono de uma plantação no Mississipi.</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1058,6 +1163,9 @@
       <c r="D45">
         <v>8.5</v>
       </c>
+      <c r="E45" t="str">
+        <v>Um misterioso estranho se junta com um bandido para proteger a uma viúva.</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -1072,6 +1180,9 @@
       <c r="D46">
         <v>8.4</v>
       </c>
+      <c r="E46" t="str">
+        <v>Um oficial do exército dos Estados Unidos no Vietnã é encarregado de assassinar a um coronel que acredita ser um deus.</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -1086,6 +1197,9 @@
       <c r="D47">
         <v>8.4</v>
       </c>
+      <c r="E47" t="str">
+        <v>Um homem com perda da memória de curto prazo tenta investigar o homicídio da sua esposa.</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -1100,6 +1214,9 @@
       <c r="D48">
         <v>8.5</v>
       </c>
+      <c r="E48" t="str">
+        <v>Diante da difícil escolha entre o amor de sua vida e o destino do universo conhecido, Paul Atreides, agora ao lado de Chani e dos Fremen, dará tudo de si para evitar o futuro terrível que só ele pode prever.</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1114,6 +1231,9 @@
       <c r="D49">
         <v>8.4</v>
       </c>
+      <c r="E49" t="str">
+        <v>Os Vingadores e seus aliados deverão sacrificar tudo em uma tentativa de derrotar o poderoso Thanos antes que sua explosão de devastação ponha fim ao universo.</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -1128,6 +1248,9 @@
       <c r="D50">
         <v>8.4</v>
       </c>
+      <c r="E50" t="str">
+        <v>Em 1984, em Berlim Oriental, um agente da polícia secreta que cuida de um escritor e sua mulher se vê cada vez mais absorvido em suas vidas.</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1142,6 +1265,9 @@
       <c r="D51">
         <v>8.4</v>
       </c>
+      <c r="E51" t="str">
+        <v>O adolescente Miles Morales se torna o Homem-Aranha de seu universo e deve se juntar a cinco indivíduos com poderes de aranha de outras dimensões para impedir uma ameaça para todas as realidades.</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -1156,6 +1282,9 @@
       <c r="D52">
         <v>8.4</v>
       </c>
+      <c r="E52" t="str">
+        <v>Um veterano advogado britânico deve defender seu cliente em um julgamento de assassinato que tem surpresa após surpresa.</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -1170,6 +1299,9 @@
       <c r="D53">
         <v>8.4</v>
       </c>
+      <c r="E53" t="str">
+        <v>Depois de se recusar a atacar uma posição inimiga, um general acusa os soldados da covardia e seu comandante deve defendê-los.</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -1184,6 +1316,9 @@
       <c r="D54">
         <v>8.4</v>
       </c>
+      <c r="E54" t="str">
+        <v>Uma família se dirige a um hotel isolado para o inverno, onde uma presença sinistra influencia a violência do pai, enquanto seu filho psíquico vê presságios horríveis do passado e do futuro.</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1198,6 +1333,9 @@
       <c r="D55">
         <v>8.4</v>
       </c>
+      <c r="E55" t="str">
+        <v>Na França ocupada pelos nazistas durante a Segunda Guerra Mundial, um plano para assassinar líderes nazistas por parte de um grupo de soldados judeus dos EUA coincide com os planos de vingança da dona de uma sala de cinema.</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1212,6 +1350,9 @@
       <c r="D56">
         <v>8.7</v>
       </c>
+      <c r="E56" t="str">
+        <v>A história da vida real do oficial do IPS Manoj Kumar Sharma e do oficial do IRS Shraddha Joshi.</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1226,6 +1367,9 @@
       <c r="D57">
         <v>8.4</v>
       </c>
+      <c r="E57" t="str">
+        <v>Ellen Ripley é salvada depois de estar dormida por 57 anos. A luna que o Nostromo visitou foi colonizada mas o contado se perdeu.</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1240,6 +1384,9 @@
       <c r="D58">
         <v>8.4</v>
       </c>
+      <c r="E58" t="str">
+        <v>Passaram-se oito anos desde a morte de Harvey Dent e o Batman, ao assumir a culpa pela morte do promotor, desapareceu. Agora, ele terá de lidar com a chegada da Mulher Gato e de Bane em Gotham City.</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1254,6 +1401,9 @@
       <c r="D59">
         <v>8.4</v>
       </c>
+      <c r="E59" t="str">
+        <v>Após os eventos devastadores de Vingadores: Guerra Infinita, o universo está em ruínas. E com a ajuda de aliados, os Vingadores se reúnem para desfazer as ações de Thanos e restaurar a ordem.</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1268,6 +1418,9 @@
       <c r="D60">
         <v>8.3</v>
       </c>
+      <c r="E60" t="str">
+        <v>Will Hunting, um zelador de uma universidade, tem habilidades para a matemática, mas precisa da ajuda de um psicólogo para encontrar seu propósito.</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1282,6 +1435,9 @@
       <c r="D61">
         <v>8.3</v>
       </c>
+      <c r="E61" t="str">
+        <v>Um general alienado provoca um potencial holocausto nuclear que uma sala de guerra cheia de políticos e generais tenta freneticamente parar.</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -1296,6 +1452,9 @@
       <c r="D62">
         <v>8.4</v>
       </c>
+      <c r="E62" t="str">
+        <v>O mundo claustrofóbico de um submarino da Segunda Guerra Mundial, cheio de tédio, sujeira e terror.</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -1310,6 +1469,9 @@
       <c r="D63">
         <v>8.3</v>
       </c>
+      <c r="E63" t="str">
+        <v>Quando sua noiva en segredo é assassinada, William Wallace comença uma revolta contra o rey Eduardo I da Inglaterra.</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -1324,6 +1486,9 @@
       <c r="D64">
         <v>8.3</v>
       </c>
+      <c r="E64" t="str">
+        <v>Um príncipe sofre com uma maldição mortal e parte em busca da cura. Ele acaba indo parar no meio da batalha entre uma cidade mineradora e os animais da floresta.</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -1338,6 +1503,9 @@
       <c r="D65">
         <v>8.3</v>
       </c>
+      <c r="E65" t="str">
+        <v>Um pai sexualmente frustrado tem uma crise existencial depois de conhecer a melhor amiga da sua filha.</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -1352,6 +1520,9 @@
       <c r="D66">
         <v>8.4</v>
       </c>
+      <c r="E66" t="str">
+        <v>Dois amigos procuram seu companheiro perdido. Eles se lembram de seus dias de faculdade e como seu amigo os inspirou a pensar de maneira diferente, mesmo quando o resto do mundo os chamava idiotas.</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -1366,6 +1537,9 @@
       <c r="D67">
         <v>8.3</v>
       </c>
+      <c r="E67" t="str">
+        <v>Um comediante falido enlouquece e se torna um assassino psicopata.</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -1380,6 +1554,9 @@
       <c r="D68">
         <v>8.4</v>
       </c>
+      <c r="E68" t="str">
+        <v>Ao cumprir uma sentença de cinco anos por um crime violento, uma criança de 12 anos processou seus pais por negligência.</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -1394,6 +1571,9 @@
       <c r="D69">
         <v>8.3</v>
       </c>
+      <c r="E69" t="str">
+        <v>Dois amigos leais crescem juntos cometendo pequenos crimes nas ruas do Lower East Side, em Manhattan, mas essa parceria com o tempo se desfaz em morte e mistério.</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -1408,6 +1588,9 @@
       <c r="D70">
         <v>8.3</v>
       </c>
+      <c r="E70" t="str">
+        <v>As utopias causadas pelo uso de drogas em quatro pessoas de Coney Island se rompem quando seus vícios as dominam.</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -1422,6 +1605,9 @@
       <c r="D71">
         <v>8.3</v>
       </c>
+      <c r="E71" t="str">
+        <v>Depois de encontrar uma arma, um jovem se une as forças da resistença russa contra os alemães na segunda guerra mundial.</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -1436,6 +1622,9 @@
       <c r="D72">
         <v>8.3</v>
       </c>
+      <c r="E72" t="str">
+        <v>Um professor vive uma vida solitária enquanto luta pela custódia de seu filho. Sua vida melhora lentamente quando ele encontra o amor e recebe boas notícias de seu filho, mas sua sorte está prestes a mudar por uma pequena mentira inocente.</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -1450,6 +1639,9 @@
       <c r="D73">
         <v>8.3</v>
       </c>
+      <c r="E73" t="str">
+        <v>Quando sua relaçao se volta complicada, um casal tenta um procedimento médico para que suas memorias sejam apagadas.</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -1464,6 +1656,9 @@
       <c r="D74">
         <v>8.3</v>
       </c>
+      <c r="E74" t="str">
+        <v>Os gêmeos viajam para o Oriente Médio para descobrir sua história familiar e cumprir os últimos desejos de sua mãe.</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -1478,6 +1673,9 @@
       <c r="D75">
         <v>8.3</v>
       </c>
+      <c r="E75" t="str">
+        <v>A história de T. E. Lawrence, o oficial inglês que conseguiu unir e liderar várias tribos árabes, durante a Primeira Guerra Mundial para lutar contra os turcos.</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -1492,6 +1690,9 @@
       <c r="D76">
         <v>8.3</v>
       </c>
+      <c r="E76" t="str">
+        <v>Quando um simples roubo de jóias dá errado, os criminosos sobreviventes começam a suspeitar que um deles é um informante da polícia.</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -1506,6 +1707,9 @@
       <c r="D77">
         <v>8.3</v>
       </c>
+      <c r="E77" t="str">
+        <v>Em 1980, um imigrante cubano se torna o maior traficante de cocaína de Miami.</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -1520,6 +1724,9 @@
       <c r="D78">
         <v>8.3</v>
       </c>
+      <c r="E78" t="str">
+        <v>Um grupo de ladrões de banco suspeitam que a polícia estejam atrás deles quando deixam uma pista no seu último roubo.</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -1534,6 +1741,9 @@
       <c r="D79">
         <v>8.3</v>
       </c>
+      <c r="E79" t="str">
+        <v>Um agente de seguros se deixa convencer de um esquema de assassinato e fraude, o que desperta a suspeita de um investigador.</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -1548,6 +1758,9 @@
       <c r="D80">
         <v>8.3</v>
       </c>
+      <c r="E80" t="str">
+        <v>Um executivo de publicidade de Nova Iorque tem que fugir quando é confundido por um agente de governo.</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -1562,6 +1775,9 @@
       <c r="D81">
         <v>8.3</v>
       </c>
+      <c r="E81" t="str">
+        <v>Quando a polícia de uma cidade alemã não consegue encontrar um assassino de crianças, outros criminosos decidem ajudar na caçada humana.</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -1576,6 +1792,9 @@
       <c r="D82">
         <v>8.2</v>
       </c>
+      <c r="E82" t="str">
+        <v>Um marinho dos Estados Unidos nota os deshumanizantes efeitos da guerra do Vietnã em seus colegas.</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -1590,6 +1809,9 @@
       <c r="D83">
         <v>8.2</v>
       </c>
+      <c r="E83" t="str">
+        <v>Um ex-policial luta contra seus demônios enquanto está obcecado por uma mulher bonita.</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -1604,6 +1826,9 @@
       <c r="D84">
         <v>8.3</v>
       </c>
+      <c r="E84" t="str">
+        <v>Amélie é uma parisiense ingênua com seu próprio senso de justiça. Ela decide ajudar as pessoas ao seu redor e, no caminho, descobre o amor.</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
@@ -1618,6 +1843,9 @@
       <c r="D85">
         <v>8.3</v>
       </c>
+      <c r="E85" t="str">
+        <v>Um casal é confrontado com uma decisão difícil, melhorar a vida de seu filho mudando-se para outro país ou ficar no Irã e cuidar de um pai que se deteriora e com Alzheimer.</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
@@ -1632,6 +1860,9 @@
       <c r="D86">
         <v>8.3</v>
       </c>
+      <c r="E86" t="str">
+        <v>Atticus Finch, um advogado no sul da era da Depressão, defende um homem negro contra uma acusação de estupro imerecida, e seus filhos contra o preconceito.</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
@@ -1646,6 +1877,9 @@
       <c r="D87">
         <v>8.2</v>
       </c>
+      <c r="E87" t="str">
+        <v>John McClane, agente do departamento de polícia de Nova York, tenta salvar sua esposa, Holly Gennaro, e outras pessoas que o terrorista alemão Hans Gruber tomou como reféns durante a festa de Natal no Nakatomi Plaza, em Los Angeles.</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
@@ -1660,6 +1894,9 @@
       <c r="D88">
         <v>8.2</v>
       </c>
+      <c r="E88" t="str">
+        <v>Dois golpistas se reúnem para obter o melhor golpe.</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
@@ -1674,6 +1911,9 @@
       <c r="D89">
         <v>8.2</v>
       </c>
+      <c r="E89" t="str">
+        <v>No futuro, um jovem líder de gang é levado para prisão e decide ser voluntário em um experimento, mas os resultados não são os esperados.</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
@@ -1688,6 +1928,9 @@
       <c r="D90">
         <v>8.2</v>
       </c>
+      <c r="E90" t="str">
+        <v>Um ladrão amante dos jogos reúne gângsteres desprezíveis, um grupo de nômades irlandeses e uma fazenda de porcos em meio a chantagens, fraudes, boxeadores, um cão faminto e um grande diamante.</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
@@ -1702,6 +1945,9 @@
       <c r="D91">
         <v>8.2</v>
       </c>
+      <c r="E91" t="str">
+        <v>Na Primeira Guerra Mundial, dois soldados britânicos recebem ordens aparentemente impossíveis de cumprir. Em uma corrida contra o tempo, eles precisam atravessar o território inimigo e entregar uma mensagem que pode salvar 1.600 homens.</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
@@ -1716,6 +1962,9 @@
       <c r="D92">
         <v>8.2</v>
       </c>
+      <c r="E92" t="str">
+        <v>A corrupção cresce em Los Angeles nos anos 50. Três policiais estão investigando uma série de assassinatos com sua própria marca de justiça.</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
@@ -1730,6 +1979,9 @@
       <c r="D93">
         <v>8.2</v>
       </c>
+      <c r="E93" t="str">
+        <v>O último secretário de Hitler relata seus últimos dias em seu bunker de Berlim no final da Segunda Guerra Mundial.</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
@@ -1744,6 +1996,9 @@
       <c r="D94">
         <v>8.2</v>
       </c>
+      <c r="E94" t="str">
+        <v>Na Itália da pós-guerra a bicicleta de um homem da classe trabalhadora é roubada. Ele e o filho partiram para encontrá-la.</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
@@ -1758,6 +2013,9 @@
       <c r="D95">
         <v>8.3</v>
       </c>
+      <c r="E95" t="str">
+        <v>O lutador Mahavir e suas filhas lutadoras procuram a gloria contra a opressão social nos jogos do Commonwealth.</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
@@ -1772,6 +2030,9 @@
       <c r="D96">
         <v>8.2</v>
       </c>
+      <c r="E96" t="str">
+        <v>Um valentão ítalo-americano se torna o motorista de um pianista afro-americano em um tour no sul dos Estados Unidos nos anos sessenta.</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
@@ -1786,6 +2047,9 @@
       <c r="D97">
         <v>8.2</v>
       </c>
+      <c r="E97" t="str">
+        <v>Um vendedor de seguros descobre que sua vida é um programa de televisão.</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
@@ -1800,6 +2064,9 @@
       <c r="D98">
         <v>8.3</v>
       </c>
+      <c r="E98" t="str">
+        <v>A vida de um dos maiores fundadores e primeiro secretário do Tesouro da América, Alexander Hamilton.</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
@@ -1814,6 +2081,9 @@
       <c r="D99">
         <v>8.2</v>
       </c>
+      <c r="E99" t="str">
+        <v>Um veterano de guerra mentalmente instável trabalha à noite como taxista na cidade de Nova York, onde a decadência e o desprezo alimentam seu desejo de ação violenta.</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
@@ -1828,6 +2098,9 @@
       <c r="D100">
         <v>8.2</v>
       </c>
+      <c r="E100" t="str">
+        <v>Após testemunhar a morte dos pais, o bilionário Bruce Wayne aprende a arte de lutar para confrontar a injustiça. Quando ele retorna a Gotham como Batman, ele deve deter uma sociedade secreta que pretende destruir a cidade.</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
@@ -1842,6 +2115,9 @@
       <c r="D101">
         <v>8.2</v>
       </c>
+      <c r="E101" t="str">
+        <v>Dois caçadores de recompensas com as mesmas intenções se reúnem para encontrar um criminoso ocidental.</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
@@ -1856,6 +2132,9 @@
       <c r="D102">
         <v>8.6</v>
       </c>
+      <c r="E102" t="str">
+        <v>A young and beautiful female teacher starts working in an all boys high school.</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
@@ -1870,6 +2149,9 @@
       <c r="D103">
         <v>8.2</v>
       </c>
+      <c r="E103" t="str">
+        <v>Em 1954, um policial federal dos Estados Unidos investiga o desaparecimento de um assassino que escapou de um hospital psiquiátrico.</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
@@ -1884,6 +2166,9 @@
       <c r="D104">
         <v>8.2</v>
       </c>
+      <c r="E104" t="str">
+        <v>Um homem recusa toda a ajuda de sua filha à medida que envelhece. Enquanto ele tenta entender o que está acontecendo ao seu redor, ele começa a duvidar dos seus entes queridos, da sua mente e até mesmo da estrutura de sua realidade.</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
@@ -1898,6 +2183,9 @@
       <c r="D105">
         <v>8.2</v>
       </c>
+      <c r="E105" t="str">
+        <v>Uma história sobre familia, religião, ódio e loucura, centrada na vida de um explorador de petróleo nos primeiros anos do negócio.</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
@@ -1912,6 +2200,9 @@
       <c r="D106">
         <v>8.2</v>
       </c>
+      <c r="E106" t="str">
+        <v>Um menino que consegue se comunicar com espíritos encontra ajuda de um psicólogo.</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
@@ -1926,6 +2217,9 @@
       <c r="D107">
         <v>8.2</v>
       </c>
+      <c r="E107" t="str">
+        <v>No Japão medieval, um senhor feudal decide abdicar e entregar seus domínios aos seus três filhos. Mas ele não é capaz de ver que esses novos poderes irão corrompê-los e levá-los a enfrentar um ao outro, e contra ele.</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
@@ -1940,6 +2234,9 @@
       <c r="D108">
         <v>8.2</v>
       </c>
+      <c r="E108" t="str">
+        <v>Uma história de ganância, dinheiro e assassinato acontece entre dois melhores amigos: um mafioso e um executivo de cassino, que competem uns com os outros por um império de jogo e pelo amor de uma socialite.</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
@@ -1954,6 +2251,9 @@
       <c r="D109">
         <v>8.2</v>
       </c>
+      <c r="E109" t="str">
+        <v>Violência e caos surgem quando um caçador se depara com uma negociação de drogas que deu errado e mais de dois milhões de dólares perto do Rio Grande.</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
@@ -1968,6 +2268,9 @@
       <c r="D110">
         <v>8.2</v>
       </c>
+      <c r="E110" t="str">
+        <v>Após mais de trinta anos de serviço como um dos melhores aviadores da Marinha, Pete Mitchell está onde pertence, ultrapassando os limites como um piloto de teste intrépido e evitando a promoção de posto que o manteria em terra.</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
@@ -1982,6 +2285,9 @@
       <c r="D111">
         <v>8.2</v>
       </c>
+      <c r="E111" t="str">
+        <v>Uma equipe de pesquisa na Antártica é caçada por um alienígena que muda de forma e assume a aparência de suas vítimas.</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
@@ -1996,6 +2302,9 @@
       <c r="D112">
         <v>8.2</v>
       </c>
+      <c r="E112" t="str">
+        <v>O atirador do Velho Oeste, William Munny, relutantemente aceita um último trabalho com a ajuda de seu antigo amigo e um jovem.</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
@@ -2010,6 +2319,9 @@
       <c r="D113">
         <v>8.2</v>
       </c>
+      <c r="E113" t="str">
+        <v>Na Espanha de 1944, a filha dum oficial do exército escapa a um mundo de fantasia.</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
@@ -2024,6 +2336,9 @@
       <c r="D114">
         <v>8.2</v>
       </c>
+      <c r="E114" t="str">
+        <v>Depois de despertar de um coma de quatro anos, uma antiga assassina busca vingança contra o grupo de assassinos que a traiu.</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
@@ -2038,6 +2353,9 @@
       <c r="D115">
         <v>8.2</v>
       </c>
+      <c r="E115" t="str">
+        <v>O único sobrevivente conta os torcidos eventos duma luta com pistolas num bote, quanfo cinco criminais eram levados pela polícia.</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
@@ -2052,6 +2370,9 @@
       <c r="D116">
         <v>8.2</v>
       </c>
+      <c r="E116" t="str">
+        <v>A vida do brilhante mas insociável matemático John Nash muda quando ele aceita um trabalho secreto em criptografia.</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
@@ -2066,6 +2387,9 @@
       <c r="D117">
         <v>8.4</v>
       </c>
+      <c r="E117" t="str">
+        <v>Um épico italiano que segue a vida de dois irmãos, das décadas de 1960 a 2000.</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
@@ -2080,6 +2404,9 @@
       <c r="D118">
         <v>8.2</v>
       </c>
+      <c r="E118" t="str">
+        <v>Prisioneiros de guerra aliados planejam uma fuga maciça de um campo alemão durante a Segunda Guerra Mundial.</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
@@ -2094,6 +2421,9 @@
       <c r="D119">
         <v>8.2</v>
       </c>
+      <c r="E119" t="str">
+        <v>Um cirurgião vitoriano resgata um homem gravemente desfigurado que é maltratado enquanto tenta sobreviver como uma atração de circo. Por trás de sua aparência monstruosa, revela-se uma pessoa de bondade, inteligência e sofisticação.</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
@@ -2108,6 +2438,9 @@
       <c r="D120">
         <v>8.2</v>
       </c>
+      <c r="E120" t="str">
+        <v>Um simples ato de bondade sempre provoca outro, mesmo em um lugar gelado e distante. Quando o novo carteiro de Smeerensburg faz amizade com o fabricante de brinquedos Klaus, seus presentes derreteram uma antiga inimizade.</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
@@ -2122,6 +2455,9 @@
       <c r="D121">
         <v>8.2</v>
       </c>
+      <c r="E121" t="str">
+        <v>Um ex-tenista decide matar a esposa para herdar o dinheiro dela e se vingar de um caso que ela havia tido. A fim de se livrar de culpas, usa um antigo colega de faculdade. Mas as coisas não vão correr como estava planeado.</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
@@ -2136,6 +2472,9 @@
       <c r="D122">
         <v>8.2</v>
       </c>
+      <c r="E122" t="str">
+        <v>Um assessor jurídico aposentado escreve um romance com a esperança de fechar um de seus antigos casos de homicídio, que permanece sem solução, e superar o amor não correspondido que sentia por seu chefe. Décadas depois, ambas as memórias continuam a persegui-lo.</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
@@ -2150,6 +2489,9 @@
       <c r="D123">
         <v>8.1</v>
       </c>
+      <c r="E123" t="str">
+        <v>Um detetive particular contratado para desmascarar um adúltero é pego em uma teia de fraude, corrupção e assassinato.</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
@@ -2164,6 +2506,9 @@
       <c r="D124">
         <v>8.1</v>
       </c>
+      <c r="E124" t="str">
+        <v>Um jogo de cartas em Londres desencadeia um confronto entre quatro amigos, plantadores de maconha, agiotas e cobradores de dívidas em uma série de eventos curiosos, tudo por algo de maria, dinheiro e duas pistolas antigas.</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
@@ -2178,6 +2523,9 @@
       <c r="D125">
         <v>8.1</v>
       </c>
+      <c r="E125" t="str">
+        <v>Em um futuro da tirania britânica, um lutador clandestino conhecido como V trama um plano para derrubá-la com a ajuda de uma jovem mulher.</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
@@ -2192,6 +2540,9 @@
       <c r="D126">
         <v>8.1</v>
       </c>
+      <c r="E126" t="str">
+        <v>A violação de uma noiva e o assassinato de seu marido samurai são lembrados desde a perspectiva de um bandido, da noiva, do fantasma do samurai e de um lenhador.</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
@@ -2206,6 +2557,9 @@
       <c r="D127">
         <v>8.1</v>
       </c>
+      <c r="E127" t="str">
+        <v>Uma mãe desafia pessoalmente as autoridades locais para resolver o assassinato de sua filha.</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
@@ -2220,6 +2574,9 @@
       <c r="D128">
         <v>8.1</v>
       </c>
+      <c r="E128" t="str">
+        <v>Um agente do FBI persegue Frank Abagnale, que antes de seus 19 anos consegue ganhar milhões de dólares fingindo ser um piloto, um médico e um advogado.</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
@@ -2234,6 +2591,9 @@
       <c r="D129">
         <v>8.1</v>
       </c>
+      <c r="E129" t="str">
+        <v>Renton, profundamente imerso no mundo das drogas em Edimburgo, tenta sair do ambiente apesar da má influência dos amigos.</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
@@ -2248,6 +2608,9 @@
       <c r="D130">
         <v>8.1</v>
       </c>
+      <c r="E130" t="str">
+        <v>Depois de resolver suas diferenças com um japonês, o comandante do campo, um coronel britânico, coopera para supervisionar a construção de uma ponte ferroviária.</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
@@ -2262,6 +2625,9 @@
       <c r="D131">
         <v>8.1</v>
       </c>
+      <c r="E131" t="str">
+        <v>A vida do boxeador Jake LaMotta, cuja violência e temperamento que o levaram até o topo dos ringues destruíram a sua vida fora deles.</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
@@ -2276,6 +2642,9 @@
       <c r="D132">
         <v>8.1</v>
       </c>
+      <c r="E132" t="str">
+        <v>Conforme a batalha entre as forças do bem e do mal no mundo bruxo aumenta de proporções, Harry Potter se aproxima cada vez mais do confronto final com Voldemort.</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
@@ -2290,6 +2659,9 @@
       <c r="D133">
         <v>8.1</v>
       </c>
+      <c r="E133" t="str">
+        <v>O crime de Jerry Lundegaard se desfaz devido à falta de sorte dele e de seus colegas e ao persistente trabalho polícia.</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
@@ -2304,6 +2676,9 @@
       <c r="D134">
         <v>8.1</v>
       </c>
+      <c r="E134" t="str">
+        <v>O filho pequeno de um exboxer alcoólatra volta para casa, onde seu pai o treina para um torneio de artes marciais mistas.</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
@@ -2318,6 +2693,9 @@
       <c r="D135">
         <v>8.1</v>
       </c>
+      <c r="E135" t="str">
+        <v>O professor de Inglés John Keating inspira a seus estudantes a ver a poesia duma perspectiva diferente.</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
@@ -2332,6 +2710,9 @@
       <c r="D136">
         <v>8.1</v>
       </c>
+      <c r="E136" t="str">
+        <v>Uma mulher determinada se prepara para se tornar numa pugilista profissional.</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
@@ -2346,6 +2727,9 @@
       <c r="D137">
         <v>8.1</v>
       </c>
+      <c r="E137" t="str">
+        <v>Quando um príncipe de Jerusalém é traído e enviado à escravidão por um amigo romano, ele recupera sua liberdade e retorna para se vingar.</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
@@ -2360,6 +2744,9 @@
       <c r="D138">
         <v>8.1</v>
       </c>
+      <c r="E138" t="str">
+        <v>Walt Kowalski, um ranzinza veterano da guerra da Coreia, tenta dar uma lição em seu vizinho quando este tentar roubar seu bem mais precioso: um Gran Torino de 1972.</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
@@ -2374,6 +2761,9 @@
       <c r="D139">
         <v>8.6</v>
       </c>
+      <c r="E139" t="str">
+        <v>O Corpo de Caçadores de Demônios mergulha no Castelo do Infinito para derrotar Muzan.</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
@@ -3127,9 +3517,2219 @@
         <v>As vidas de dois assassinos da máfia, um boxeador, um gângster e sua esposa, e um par de bandidos se entrelaçam em quatro histórias de violência e redenção.</v>
       </c>
     </row>
+    <row r="192">
+      <c r="A192" t="str">
+        <v>Três Homens em Conflito</v>
+      </c>
+      <c r="B192">
+        <v>1966</v>
+      </c>
+      <c r="C192" t="str">
+        <v>2h 41m</v>
+      </c>
+      <c r="D192">
+        <v>8.8</v>
+      </c>
+      <c r="E192" t="str">
+        <v>Um impostor se junta com dois homens para encontrar fortuna num remoto cemitério.</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="str">
+        <v>Forrest Gump: O Contador de Histórias</v>
+      </c>
+      <c r="B193">
+        <v>1994</v>
+      </c>
+      <c r="C193" t="str">
+        <v>2h 22m</v>
+      </c>
+      <c r="D193">
+        <v>8.8</v>
+      </c>
+      <c r="E193" t="str">
+        <v>Os governos dos presidentes Kennedy e Johnson, os eventos do Vietnã e Watergate e outras histórias são mostradas através da perspectiva de um homem do Alabama com baixo quociente intelectual.</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="str">
+        <v>O Senhor dos Anéis: As Duas Torres</v>
+      </c>
+      <c r="B194">
+        <v>2002</v>
+      </c>
+      <c r="C194" t="str">
+        <v>2h 59m</v>
+      </c>
+      <c r="D194">
+        <v>8.8</v>
+      </c>
+      <c r="E194" t="str">
+        <v>Enquanto Frodo e Sam estão perto de Mordor com a ajuda de Gollum, a divida comunhão luta contra Saruman e os Isengards.</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="str">
+        <v>Clube da Luta</v>
+      </c>
+      <c r="B195">
+        <v>1999</v>
+      </c>
+      <c r="C195" t="str">
+        <v>2h 19m</v>
+      </c>
+      <c r="D195">
+        <v>8.8</v>
+      </c>
+      <c r="E195" t="str">
+        <v>Um trabalhador de escritório e um fabricante de sabonetes formam um clube de luta clandestino que evolui para algo muito maior.</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="str">
+        <v>A Origem</v>
+      </c>
+      <c r="B196">
+        <v>2010</v>
+      </c>
+      <c r="C196" t="str">
+        <v>2h 28m</v>
+      </c>
+      <c r="D196">
+        <v>8.8</v>
+      </c>
+      <c r="E196" t="str">
+        <v>Um ladrão que rouba segredos corporativos através da tecnologia de entrar no subconsciente recebe a tarefa inversa de plantar uma idéia na mente do diretor de uma grande empresa.</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="str">
+        <v>Matrix</v>
+      </c>
+      <c r="B197">
+        <v>1999</v>
+      </c>
+      <c r="C197" t="str">
+        <v>2h 16m</v>
+      </c>
+      <c r="D197">
+        <v>8.7</v>
+      </c>
+      <c r="E197" t="str">
+        <v>Um hacker aprende com os misteriosos rebeldes sobre a verdadeira natureza de sua realidade e seu papel na guerra contra seus controladores.</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="str">
+        <v>Os Bons Companheiros</v>
+      </c>
+      <c r="B198">
+        <v>1990</v>
+      </c>
+      <c r="C198" t="str">
+        <v>2h 25m</v>
+      </c>
+      <c r="D198">
+        <v>8.7</v>
+      </c>
+      <c r="E198" t="str">
+        <v>A historia do Henry Hill e sua vida na máfia, sua relação com sua esposa Karen Hill e seus colegas da máfia Jimmy Conway e Tommy DeVito no sindicato italo-americano do crime.</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="str">
+        <v>Interestelar</v>
+      </c>
+      <c r="B199">
+        <v>2014</v>
+      </c>
+      <c r="C199" t="str">
+        <v>2h 49m</v>
+      </c>
+      <c r="D199">
+        <v>8.7</v>
+      </c>
+      <c r="E199" t="str">
+        <v>Uma equipe de exploradores viaja através de um buraco de minhoca no espaço, na tentativa de garantir a sobrevivência da humanidade.</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="str">
+        <v>Um Estranho no Ninho</v>
+      </c>
+      <c r="B200">
+        <v>1975</v>
+      </c>
+      <c r="C200" t="str">
+        <v>2h 13m</v>
+      </c>
+      <c r="D200">
+        <v>8.7</v>
+      </c>
+      <c r="E200" t="str">
+        <v>Um criminoso alega insanidade para ser enviado a um centro de saúde mental, onde se rebela contra a opressiva enfermeira e mobiliza os pacientes a quem ela atemoriza.</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="str">
+        <v>Seven - Os Sete Crimes Capitais</v>
+      </c>
+      <c r="B201">
+        <v>1995</v>
+      </c>
+      <c r="C201" t="str">
+        <v>2h 7m</v>
+      </c>
+      <c r="D201">
+        <v>8.6</v>
+      </c>
+      <c r="E201" t="str">
+        <v>Dois detetives, um novato e um veterano, perseguem um assassino em série que usa os sete pecados capitais como motivos.</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="str">
+        <v>O Silêncio dos Inocentes</v>
+      </c>
+      <c r="B202">
+        <v>1991</v>
+      </c>
+      <c r="C202" t="str">
+        <v>1h 58m</v>
+      </c>
+      <c r="D202">
+        <v>8.6</v>
+      </c>
+      <c r="E202" t="str">
+        <v>Uma jovem deve receber a ajuda de um assassino canibal manipulador e preso para ajudar a capturar outro assassino em série, um louco que ataca suas vítimas.</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="str">
+        <v>Os Sete Samurais</v>
+      </c>
+      <c r="B203">
+        <v>1954</v>
+      </c>
+      <c r="C203" t="str">
+        <v>3h 27m</v>
+      </c>
+      <c r="D203">
+        <v>8.6</v>
+      </c>
+      <c r="E203" t="str">
+        <v>Uma aldeia pobre sob a ameaça de bandidos recruta sete samurais para ajudá-los a se defenderem.</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="str">
+        <v>O Resgate do Soldado Ryan</v>
+      </c>
+      <c r="B204">
+        <v>1998</v>
+      </c>
+      <c r="C204" t="str">
+        <v>2h 49m</v>
+      </c>
+      <c r="D204">
+        <v>8.6</v>
+      </c>
+      <c r="E204" t="str">
+        <v>Depois de chegar a Normandía, um grupo de soldados precisa encontrar o único irmão vivo de três que morreram na guerra.</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="str">
+        <v>À Espera de um Milagre</v>
+      </c>
+      <c r="B205">
+        <v>1999</v>
+      </c>
+      <c r="C205" t="str">
+        <v>3h 9m</v>
+      </c>
+      <c r="D205">
+        <v>8.6</v>
+      </c>
+      <c r="E205" t="str">
+        <v>As vidas dos guardas de corredor da morte são afetadas por um dos detidos: um homem afro-americano acusado pelo assassinato e estupro de uma criança, mas com um presente misterioso.</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="str">
+        <v>Cidade de Deus</v>
+      </c>
+      <c r="B206">
+        <v>2002</v>
+      </c>
+      <c r="C206" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D206">
+        <v>8.6</v>
+      </c>
+      <c r="E206" t="str">
+        <v>Os caminhos de duas crianças divergem nas favelas do Rio, enquanto um se esforça para se tornar um fotógrafo e o outro um chefe do tráfico.</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="str">
+        <v>O Exterminador do Futuro 2: O Julgamento Final</v>
+      </c>
+      <c r="B207">
+        <v>1991</v>
+      </c>
+      <c r="C207" t="str">
+        <v>2h 17m</v>
+      </c>
+      <c r="D207">
+        <v>8.6</v>
+      </c>
+      <c r="E207" t="str">
+        <v>Um ciborgue, idêntico ao que falhou em matar Sarah Connor, agora deve proteger o filho de dez anos dela, John, de um ciborgue ainda mais avançado e poderoso.</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="str">
+        <v>Star Wars: Episódio IV - Uma Nova Esperança</v>
+      </c>
+      <c r="B208">
+        <v>1977</v>
+      </c>
+      <c r="C208" t="str">
+        <v>2h 1m</v>
+      </c>
+      <c r="D208">
+        <v>8.6</v>
+      </c>
+      <c r="E208" t="str">
+        <v>Luke Skywalker une forças com um cavaleiro Jedi, um piloto arrogante, um Wookiee e dois andróides para salvar a galáxia da estação de batalha destruidora do Império, enquanto tenta resgatar a Princesa Leia do misterioso Darth Vader.</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="str">
+        <v>O Pianista</v>
+      </c>
+      <c r="B209">
+        <v>2002</v>
+      </c>
+      <c r="C209" t="str">
+        <v>2h 30m</v>
+      </c>
+      <c r="D209">
+        <v>8.5</v>
+      </c>
+      <c r="E209" t="str">
+        <v>Um musico judeu luta para sobreviver a destruição de Varsóvia durante a segunda guerra mundial.</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="str">
+        <v>Gladiador</v>
+      </c>
+      <c r="B210">
+        <v>2000</v>
+      </c>
+      <c r="C210" t="str">
+        <v>2h 35m</v>
+      </c>
+      <c r="D210">
+        <v>8.5</v>
+      </c>
+      <c r="E210" t="str">
+        <v>Um general romano planeja a melhor vingança contra o imperador corrupto que matou sua familia e o fez escravo.</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="str">
+        <v>Parasita</v>
+      </c>
+      <c r="B211">
+        <v>2019</v>
+      </c>
+      <c r="C211" t="str">
+        <v>2h 12m</v>
+      </c>
+      <c r="D211">
+        <v>8.5</v>
+      </c>
+      <c r="E211" t="str">
+        <v>Desempregados, a família de Ki-taek (Song Kang-ho) nutre um interesse peculiar pela família Park até que eles se veem presos em um inesperado incidente.</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="str">
+        <v>Psicose</v>
+      </c>
+      <c r="B212">
+        <v>1960</v>
+      </c>
+      <c r="C212" t="str">
+        <v>1h 49m</v>
+      </c>
+      <c r="D212">
+        <v>8.5</v>
+      </c>
+      <c r="E212" t="str">
+        <v>Uma secretária de Phoenix desvia dinheiro de um cliente de sua empresa, foge e vai a um motel remoto gerido por um jovem sob o domínio da mãe.</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="str">
+        <v>Túmulo dos Vagalumes</v>
+      </c>
+      <c r="B213">
+        <v>1988</v>
+      </c>
+      <c r="C213" t="str">
+        <v>1h 28m</v>
+      </c>
+      <c r="D213">
+        <v>8.5</v>
+      </c>
+      <c r="E213" t="str">
+        <v>Um menino e sua irmã tentam sobreviver no Japão durante a Segunda Guerra Mundial.</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="str">
+        <v>Os Infiltrados</v>
+      </c>
+      <c r="B214">
+        <v>2006</v>
+      </c>
+      <c r="C214" t="str">
+        <v>2h 31m</v>
+      </c>
+      <c r="D214">
+        <v>8.5</v>
+      </c>
+      <c r="E214" t="str">
+        <v>Um policial disfarçado e um espião estão tentando se identificar enquanto se infiltram em uma gangue irlandesa no sul de Boston.</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="str">
+        <v>Whiplash: Em Busca da Perfeição</v>
+      </c>
+      <c r="B215">
+        <v>2014</v>
+      </c>
+      <c r="C215" t="str">
+        <v>1h 46m</v>
+      </c>
+      <c r="D215">
+        <v>8.5</v>
+      </c>
+      <c r="E215" t="str">
+        <v>Um jovem e promissor baterista se matricula em um conservatório de música onde seus sonhos são guiados por um instrutor que não pára por nada para perceber o potencial de um aluno.</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="str">
+        <v>Harakiri</v>
+      </c>
+      <c r="B216">
+        <v>1962</v>
+      </c>
+      <c r="C216" t="str">
+        <v>2h 13m</v>
+      </c>
+      <c r="D216">
+        <v>8.6</v>
+      </c>
+      <c r="E216" t="str">
+        <v>Um velho samurai ronin chega à casa de um senhor feudal e pede um lugar honroso para cometer suicídio. Mas quando o ronin pede um samurai mais jovem que chegou antes, os eventos seguem um curso inesperado.</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="str">
+        <v>O Grande Truque</v>
+      </c>
+      <c r="B217">
+        <v>2006</v>
+      </c>
+      <c r="C217" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D217">
+        <v>8.5</v>
+      </c>
+      <c r="E217" t="str">
+        <v>Depois de um trágico acidente, dois magos do palco se engajam em uma batalha para criar a ilusão final enquanto sacrificam tudo o que têm para enganar um ao outro.</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="str">
+        <v>A Outra História Americana</v>
+      </c>
+      <c r="B218">
+        <v>1998</v>
+      </c>
+      <c r="C218" t="str">
+        <v>1h 59m</v>
+      </c>
+      <c r="D218">
+        <v>8.5</v>
+      </c>
+      <c r="E218" t="str">
+        <v>Um neonazista tenta evitar que seu irmão mais novo tome o mesmo caminho errado que ele.</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="str">
+        <v>O Profissional</v>
+      </c>
+      <c r="B219">
+        <v>1994</v>
+      </c>
+      <c r="C219" t="str">
+        <v>1h 50m</v>
+      </c>
+      <c r="D219">
+        <v>8.5</v>
+      </c>
+      <c r="E219" t="str">
+        <v>Mathilda, uma menina de 12 anos é levada por Léon, um assassino profissional, depois que sua família é assassinada. Léon e Mathilda formam uma relação incomum, desde que ela se torna sua protegida.</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="str">
+        <v>Homem-Aranha: Através do Aranhaverso</v>
+      </c>
+      <c r="B220">
+        <v>2023</v>
+      </c>
+      <c r="C220" t="str">
+        <v>2h 20m</v>
+      </c>
+      <c r="D220">
+        <v>8.5</v>
+      </c>
+      <c r="E220" t="str">
+        <v>Viajando pelo multiverso, Miles Morales conhece um novo time de Pessoas-Aranha, formado por heróis de diversas dimensões. Mas quando os heróis entram em conflito sobre como lidar com uma nova ameaça, Miles se vê em um impasse.</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="str">
+        <v>Cinema Paradiso</v>
+      </c>
+      <c r="B221">
+        <v>1988</v>
+      </c>
+      <c r="C221" t="str">
+        <v>2h 54m</v>
+      </c>
+      <c r="D221">
+        <v>8.5</v>
+      </c>
+      <c r="E221" t="str">
+        <v>Um diretor de cinema lembra como, em sua infância, ele se apaixonou pelo cinema de sua cidade e iniciou uma profunda amizade com o projecionista.</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="str">
+        <v>Intocáveis</v>
+      </c>
+      <c r="B222">
+        <v>2011</v>
+      </c>
+      <c r="C222" t="str">
+        <v>1h 52m</v>
+      </c>
+      <c r="D222">
+        <v>8.5</v>
+      </c>
+      <c r="E222" t="str">
+        <v>Depois de ficar tetraplégico num acidente, um aristocrata contrata um jovem de um bairro pobre para cuidar dele.</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="str">
+        <v>Os Suspeitos</v>
+      </c>
+      <c r="B223">
+        <v>1995</v>
+      </c>
+      <c r="C223" t="str">
+        <v>1h 46m</v>
+      </c>
+      <c r="D223">
+        <v>8.5</v>
+      </c>
+      <c r="E223" t="str">
+        <v>O único sobrevivente conta os torcidos eventos duma luta com pistolas num bote, quanfo cinco criminais eram levados pela polícia.</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="str">
+        <v>Alien - O 8º Passageiro</v>
+      </c>
+      <c r="B224">
+        <v>1979</v>
+      </c>
+      <c r="C224" t="str">
+        <v>1h 57m</v>
+      </c>
+      <c r="D224">
+        <v>8.5</v>
+      </c>
+      <c r="E224" t="str">
+        <v>Depois de investigar uma transmissão misteriosa de origem desconhecida, a tripulação de uma nave espacial comercial encontra uma forma de vida mortal.</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="str">
+        <v>Janela Indiscreta</v>
+      </c>
+      <c r="B225">
+        <v>1954</v>
+      </c>
+      <c r="C225" t="str">
+        <v>1h 52m</v>
+      </c>
+      <c r="D225">
+        <v>8.5</v>
+      </c>
+      <c r="E225" t="str">
+        <v>Um fotógrafo em uma cadeira de rodas espiona seus vizinhos pela janela de seu apartamento e está convencido de que um deles cometeu um assassinato.</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="str">
+        <v>Django Livre</v>
+      </c>
+      <c r="B226">
+        <v>2012</v>
+      </c>
+      <c r="C226" t="str">
+        <v>2h 45m</v>
+      </c>
+      <c r="D226">
+        <v>8.5</v>
+      </c>
+      <c r="E226" t="str">
+        <v>Com a ajuda de um caçador de recompensas alemão, um escravo libertado sai para resgatar sua esposa de um brutal dono de uma plantação no Mississipi.</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="str">
+        <v>Era uma Vez no Oeste</v>
+      </c>
+      <c r="B227">
+        <v>1968</v>
+      </c>
+      <c r="C227" t="str">
+        <v>2h 46m</v>
+      </c>
+      <c r="D227">
+        <v>8.5</v>
+      </c>
+      <c r="E227" t="str">
+        <v>Um misterioso estranho se junta com um bandido para proteger a uma viúva.</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="str">
+        <v>Apocalypse Now</v>
+      </c>
+      <c r="B228">
+        <v>1979</v>
+      </c>
+      <c r="C228" t="str">
+        <v>2h 27m</v>
+      </c>
+      <c r="D228">
+        <v>8.4</v>
+      </c>
+      <c r="E228" t="str">
+        <v>Um oficial do exército dos Estados Unidos no Vietnã é encarregado de assassinar a um coronel que acredita ser um deus.</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="str">
+        <v>Amnésia</v>
+      </c>
+      <c r="B229">
+        <v>2000</v>
+      </c>
+      <c r="C229" t="str">
+        <v>1h 53m</v>
+      </c>
+      <c r="D229">
+        <v>8.4</v>
+      </c>
+      <c r="E229" t="str">
+        <v>Um homem com perda da memória de curto prazo tenta investigar o homicídio da sua esposa.</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="str">
+        <v>Duna: Parte 2</v>
+      </c>
+      <c r="B230">
+        <v>2024</v>
+      </c>
+      <c r="C230" t="str">
+        <v>2h 46m</v>
+      </c>
+      <c r="D230">
+        <v>8.5</v>
+      </c>
+      <c r="E230" t="str">
+        <v>Diante da difícil escolha entre o amor de sua vida e o destino do universo conhecido, Paul Atreides, agora ao lado de Chani e dos Fremen, dará tudo de si para evitar o futuro terrível que só ele pode prever.</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="str">
+        <v>Vingadores: Guerra Infinita</v>
+      </c>
+      <c r="B231">
+        <v>2018</v>
+      </c>
+      <c r="C231" t="str">
+        <v>2h 29m</v>
+      </c>
+      <c r="D231">
+        <v>8.4</v>
+      </c>
+      <c r="E231" t="str">
+        <v>Os Vingadores e seus aliados deverão sacrificar tudo em uma tentativa de derrotar o poderoso Thanos antes que sua explosão de devastação ponha fim ao universo.</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="str">
+        <v>A Vida dos Outros</v>
+      </c>
+      <c r="B232">
+        <v>2006</v>
+      </c>
+      <c r="C232" t="str">
+        <v>2h 17m</v>
+      </c>
+      <c r="D232">
+        <v>8.4</v>
+      </c>
+      <c r="E232" t="str">
+        <v>Em 1984, em Berlim Oriental, um agente da polícia secreta que cuida de um escritor e sua mulher se vê cada vez mais absorvido em suas vidas.</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="str">
+        <v>Homem-Aranha: No Aranhaverso</v>
+      </c>
+      <c r="B233">
+        <v>2018</v>
+      </c>
+      <c r="C233" t="str">
+        <v>1h 57m</v>
+      </c>
+      <c r="D233">
+        <v>8.4</v>
+      </c>
+      <c r="E233" t="str">
+        <v>O adolescente Miles Morales se torna o Homem-Aranha de seu universo e deve se juntar a cinco indivíduos com poderes de aranha de outras dimensões para impedir uma ameaça para todas as realidades.</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="str">
+        <v>Testemunha de Acusação</v>
+      </c>
+      <c r="B234">
+        <v>1957</v>
+      </c>
+      <c r="C234" t="str">
+        <v>1h 56m</v>
+      </c>
+      <c r="D234">
+        <v>8.4</v>
+      </c>
+      <c r="E234" t="str">
+        <v>Um veterano advogado britânico deve defender seu cliente em um julgamento de assassinato que tem surpresa após surpresa.</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="str">
+        <v>Glória Feita de Sangue</v>
+      </c>
+      <c r="B235">
+        <v>1957</v>
+      </c>
+      <c r="C235" t="str">
+        <v>1h 28m</v>
+      </c>
+      <c r="D235">
+        <v>8.4</v>
+      </c>
+      <c r="E235" t="str">
+        <v>Depois de se recusar a atacar uma posição inimiga, um general acusa os soldados da covardia e seu comandante deve defendê-los.</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="str">
+        <v>O Iluminado</v>
+      </c>
+      <c r="B236">
+        <v>1980</v>
+      </c>
+      <c r="C236" t="str">
+        <v>2h 26m</v>
+      </c>
+      <c r="D236">
+        <v>8.4</v>
+      </c>
+      <c r="E236" t="str">
+        <v>Uma família se dirige a um hotel isolado para o inverno, onde uma presença sinistra influencia a violência do pai, enquanto seu filho psíquico vê presságios horríveis do passado e do futuro.</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="str">
+        <v>Bastardos Inglórios</v>
+      </c>
+      <c r="B237">
+        <v>2009</v>
+      </c>
+      <c r="C237" t="str">
+        <v>2h 33m</v>
+      </c>
+      <c r="D237">
+        <v>8.4</v>
+      </c>
+      <c r="E237" t="str">
+        <v>Na França ocupada pelos nazistas durante a Segunda Guerra Mundial, um plano para assassinar líderes nazistas por parte de um grupo de soldados judeus dos EUA coincide com os planos de vingança da dona de uma sala de cinema.</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="str">
+        <v>Repetente</v>
+      </c>
+      <c r="B238">
+        <v>2023</v>
+      </c>
+      <c r="C238" t="str">
+        <v>2h 27m</v>
+      </c>
+      <c r="D238">
+        <v>8.7</v>
+      </c>
+      <c r="E238" t="str">
+        <v>A história da vida real do oficial do IPS Manoj Kumar Sharma e do oficial do IRS Shraddha Joshi.</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="str">
+        <v>Aliens: O Resgate</v>
+      </c>
+      <c r="B239">
+        <v>1986</v>
+      </c>
+      <c r="C239" t="str">
+        <v>2h 17m</v>
+      </c>
+      <c r="D239">
+        <v>8.4</v>
+      </c>
+      <c r="E239" t="str">
+        <v>Ellen Ripley é salvada depois de estar dormida por 57 anos. A luna que o Nostromo visitou foi colonizada mas o contado se perdeu.</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="str">
+        <v>Batman: O Cavaleiro das Trevas Ressurge</v>
+      </c>
+      <c r="B240">
+        <v>2012</v>
+      </c>
+      <c r="C240" t="str">
+        <v>2h 44m</v>
+      </c>
+      <c r="D240">
+        <v>8.4</v>
+      </c>
+      <c r="E240" t="str">
+        <v>Passaram-se oito anos desde a morte de Harvey Dent e o Batman, ao assumir a culpa pela morte do promotor, desapareceu. Agora, ele terá de lidar com a chegada da Mulher Gato e de Bane em Gotham City.</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="str">
+        <v>Vingadores: Ultimato</v>
+      </c>
+      <c r="B241">
+        <v>2019</v>
+      </c>
+      <c r="C241" t="str">
+        <v>3h 1m</v>
+      </c>
+      <c r="D241">
+        <v>8.4</v>
+      </c>
+      <c r="E241" t="str">
+        <v>Após os eventos devastadores de Vingadores: Guerra Infinita, o universo está em ruínas. E com a ajuda de aliados, os Vingadores se reúnem para desfazer as ações de Thanos e restaurar a ordem.</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="str">
+        <v>Gênio Indomável</v>
+      </c>
+      <c r="B242">
+        <v>1997</v>
+      </c>
+      <c r="C242" t="str">
+        <v>2h 6m</v>
+      </c>
+      <c r="D242">
+        <v>8.3</v>
+      </c>
+      <c r="E242" t="str">
+        <v>Will Hunting, um zelador de uma universidade, tem habilidades para a matemática, mas precisa da ajuda de um psicólogo para encontrar seu propósito.</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="str">
+        <v>Dr. Fantástico</v>
+      </c>
+      <c r="B243">
+        <v>1964</v>
+      </c>
+      <c r="C243" t="str">
+        <v>1h 35m</v>
+      </c>
+      <c r="D243">
+        <v>8.3</v>
+      </c>
+      <c r="E243" t="str">
+        <v>Um general alienado provoca um potencial holocausto nuclear que uma sala de guerra cheia de políticos e generais tenta freneticamente parar.</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="str">
+        <v>O Barco: Inferno no Mar</v>
+      </c>
+      <c r="B244">
+        <v>1981</v>
+      </c>
+      <c r="C244" t="str">
+        <v>2h 29m</v>
+      </c>
+      <c r="D244">
+        <v>8.4</v>
+      </c>
+      <c r="E244" t="str">
+        <v>O mundo claustrofóbico de um submarino da Segunda Guerra Mundial, cheio de tédio, sujeira e terror.</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="str">
+        <v>Coração Valente</v>
+      </c>
+      <c r="B245">
+        <v>1995</v>
+      </c>
+      <c r="C245" t="str">
+        <v>2h 58m</v>
+      </c>
+      <c r="D245">
+        <v>8.3</v>
+      </c>
+      <c r="E245" t="str">
+        <v>Quando sua noiva en segredo é assassinada, William Wallace comença uma revolta contra o rey Eduardo I da Inglaterra.</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="str">
+        <v>Princesa Mononoke</v>
+      </c>
+      <c r="B246">
+        <v>1997</v>
+      </c>
+      <c r="C246" t="str">
+        <v>2h 13m</v>
+      </c>
+      <c r="D246">
+        <v>8.3</v>
+      </c>
+      <c r="E246" t="str">
+        <v>Um príncipe sofre com uma maldição mortal e parte em busca da cura. Ele acaba indo parar no meio da batalha entre uma cidade mineradora e os animais da floresta.</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="str">
+        <v>Beleza Americana</v>
+      </c>
+      <c r="B247">
+        <v>1999</v>
+      </c>
+      <c r="C247" t="str">
+        <v>2h 2m</v>
+      </c>
+      <c r="D247">
+        <v>8.3</v>
+      </c>
+      <c r="E247" t="str">
+        <v>Um pai sexualmente frustrado tem uma crise existencial depois de conhecer a melhor amiga da sua filha.</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="str">
+        <v>3 Idiotas</v>
+      </c>
+      <c r="B248">
+        <v>2009</v>
+      </c>
+      <c r="C248" t="str">
+        <v>2h 50m</v>
+      </c>
+      <c r="D248">
+        <v>8.4</v>
+      </c>
+      <c r="E248" t="str">
+        <v>Dois amigos procuram seu companheiro perdido. Eles se lembram de seus dias de faculdade e como seu amigo os inspirou a pensar de maneira diferente, mesmo quando o resto do mundo os chamava idiotas.</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="str">
+        <v>Coringa</v>
+      </c>
+      <c r="B249">
+        <v>2019</v>
+      </c>
+      <c r="C249" t="str">
+        <v>2h 2m</v>
+      </c>
+      <c r="D249">
+        <v>8.3</v>
+      </c>
+      <c r="E249" t="str">
+        <v>Um comediante falido enlouquece e se torna um assassino psicopata.</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="str">
+        <v>Cafarnaum</v>
+      </c>
+      <c r="B250">
+        <v>2018</v>
+      </c>
+      <c r="C250" t="str">
+        <v>2h 6m</v>
+      </c>
+      <c r="D250">
+        <v>8.4</v>
+      </c>
+      <c r="E250" t="str">
+        <v>Ao cumprir uma sentença de cinco anos por um crime violento, uma criança de 12 anos processou seus pais por negligência.</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="str">
+        <v>Era uma Vez na América</v>
+      </c>
+      <c r="B251">
+        <v>1984</v>
+      </c>
+      <c r="C251" t="str">
+        <v>3h 49m</v>
+      </c>
+      <c r="D251">
+        <v>8.3</v>
+      </c>
+      <c r="E251" t="str">
+        <v>Dois amigos leais crescem juntos cometendo pequenos crimes nas ruas do Lower East Side, em Manhattan, mas essa parceria com o tempo se desfaz em morte e mistério.</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="str">
+        <v>Réquiem para um Sonho</v>
+      </c>
+      <c r="B252">
+        <v>2000</v>
+      </c>
+      <c r="C252" t="str">
+        <v>1h 42m</v>
+      </c>
+      <c r="D252">
+        <v>8.3</v>
+      </c>
+      <c r="E252" t="str">
+        <v>As utopias causadas pelo uso de drogas em quatro pessoas de Coney Island se rompem quando seus vícios as dominam.</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="str">
+        <v>Vá e Veja</v>
+      </c>
+      <c r="B253">
+        <v>1985</v>
+      </c>
+      <c r="C253" t="str">
+        <v>2h 22m</v>
+      </c>
+      <c r="D253">
+        <v>8.3</v>
+      </c>
+      <c r="E253" t="str">
+        <v>Depois de encontrar uma arma, um jovem se une as forças da resistença russa contra os alemães na segunda guerra mundial.</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="str">
+        <v>A Caça</v>
+      </c>
+      <c r="B254">
+        <v>2012</v>
+      </c>
+      <c r="C254" t="str">
+        <v>1h 55m</v>
+      </c>
+      <c r="D254">
+        <v>8.3</v>
+      </c>
+      <c r="E254" t="str">
+        <v>Um professor vive uma vida solitária enquanto luta pela custódia de seu filho. Sua vida melhora lentamente quando ele encontra o amor e recebe boas notícias de seu filho, mas sua sorte está prestes a mudar por uma pequena mentira inocente.</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="str">
+        <v>Brilho Eterno de uma Mente sem Lembranças</v>
+      </c>
+      <c r="B255">
+        <v>2004</v>
+      </c>
+      <c r="C255" t="str">
+        <v>1h 48m</v>
+      </c>
+      <c r="D255">
+        <v>8.3</v>
+      </c>
+      <c r="E255" t="str">
+        <v>Quando sua relaçao se volta complicada, um casal tenta um procedimento médico para que suas memorias sejam apagadas.</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="str">
+        <v>Incêndios</v>
+      </c>
+      <c r="B256">
+        <v>2010</v>
+      </c>
+      <c r="C256" t="str">
+        <v>2h 11m</v>
+      </c>
+      <c r="D256">
+        <v>8.3</v>
+      </c>
+      <c r="E256" t="str">
+        <v>Os gêmeos viajam para o Oriente Médio para descobrir sua história familiar e cumprir os últimos desejos de sua mãe.</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="str">
+        <v>Lawrence da Arábia</v>
+      </c>
+      <c r="B257">
+        <v>1962</v>
+      </c>
+      <c r="C257" t="str">
+        <v>3h 47m</v>
+      </c>
+      <c r="D257">
+        <v>8.3</v>
+      </c>
+      <c r="E257" t="str">
+        <v>A história de T. E. Lawrence, o oficial inglês que conseguiu unir e liderar várias tribos árabes, durante a Primeira Guerra Mundial para lutar contra os turcos.</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="str">
+        <v>Cães de Aluguel</v>
+      </c>
+      <c r="B258">
+        <v>1992</v>
+      </c>
+      <c r="C258" t="str">
+        <v>1h 39m</v>
+      </c>
+      <c r="D258">
+        <v>8.3</v>
+      </c>
+      <c r="E258" t="str">
+        <v>Quando um simples roubo de jóias dá errado, os criminosos sobreviventes começam a suspeitar que um deles é um informante da polícia.</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="str">
+        <v>Scarface</v>
+      </c>
+      <c r="B259">
+        <v>1983</v>
+      </c>
+      <c r="C259" t="str">
+        <v>2h 50m</v>
+      </c>
+      <c r="D259">
+        <v>8.3</v>
+      </c>
+      <c r="E259" t="str">
+        <v>Em 1980, um imigrante cubano se torna o maior traficante de cocaína de Miami.</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="str">
+        <v>Fogo Contra Fogo</v>
+      </c>
+      <c r="B260">
+        <v>1995</v>
+      </c>
+      <c r="C260" t="str">
+        <v>2h 50m</v>
+      </c>
+      <c r="D260">
+        <v>8.3</v>
+      </c>
+      <c r="E260" t="str">
+        <v>Um grupo de ladrões de banco suspeitam que a polícia estejam atrás deles quando deixam uma pista no seu último roubo.</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="str">
+        <v>Pacto de Sangue</v>
+      </c>
+      <c r="B261">
+        <v>1944</v>
+      </c>
+      <c r="C261" t="str">
+        <v>1h 47m</v>
+      </c>
+      <c r="D261">
+        <v>8.3</v>
+      </c>
+      <c r="E261" t="str">
+        <v>Um agente de seguros se deixa convencer de um esquema de assassinato e fraude, o que desperta a suspeita de um investigador.</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="str">
+        <v>Intriga Internacional</v>
+      </c>
+      <c r="B262">
+        <v>1959</v>
+      </c>
+      <c r="C262" t="str">
+        <v>2h 16m</v>
+      </c>
+      <c r="D262">
+        <v>8.3</v>
+      </c>
+      <c r="E262" t="str">
+        <v>Um executivo de publicidade de Nova Iorque tem que fugir quando é confundido por um agente de governo.</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="str">
+        <v>M, o Vampiro de Dusseldorf</v>
+      </c>
+      <c r="B263">
+        <v>1931</v>
+      </c>
+      <c r="C263" t="str">
+        <v>1h 57m</v>
+      </c>
+      <c r="D263">
+        <v>8.3</v>
+      </c>
+      <c r="E263" t="str">
+        <v>Quando a polícia de uma cidade alemã não consegue encontrar um assassino de crianças, outros criminosos decidem ajudar na caçada humana.</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="str">
+        <v>Nascido para Matar</v>
+      </c>
+      <c r="B264">
+        <v>1987</v>
+      </c>
+      <c r="C264" t="str">
+        <v>1h 56m</v>
+      </c>
+      <c r="D264">
+        <v>8.2</v>
+      </c>
+      <c r="E264" t="str">
+        <v>Um marinho dos Estados Unidos nota os deshumanizantes efeitos da guerra do Vietnã em seus colegas.</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="str">
+        <v>Um Corpo que Cai</v>
+      </c>
+      <c r="B265">
+        <v>1958</v>
+      </c>
+      <c r="C265" t="str">
+        <v>2h 8m</v>
+      </c>
+      <c r="D265">
+        <v>8.2</v>
+      </c>
+      <c r="E265" t="str">
+        <v>Um ex-policial luta contra seus demônios enquanto está obcecado por uma mulher bonita.</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="str">
+        <v>O Fabuloso Destino de Amélie Poulain</v>
+      </c>
+      <c r="B266">
+        <v>2001</v>
+      </c>
+      <c r="C266" t="str">
+        <v>2h 2m</v>
+      </c>
+      <c r="D266">
+        <v>8.3</v>
+      </c>
+      <c r="E266" t="str">
+        <v>Amélie é uma parisiense ingênua com seu próprio senso de justiça. Ela decide ajudar as pessoas ao seu redor e, no caminho, descobre o amor.</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="str">
+        <v>A Separação</v>
+      </c>
+      <c r="B267">
+        <v>2011</v>
+      </c>
+      <c r="C267" t="str">
+        <v>2h 3m</v>
+      </c>
+      <c r="D267">
+        <v>8.3</v>
+      </c>
+      <c r="E267" t="str">
+        <v>Um casal é confrontado com uma decisão difícil, melhorar a vida de seu filho mudando-se para outro país ou ficar no Irã e cuidar de um pai que se deteriora e com Alzheimer.</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="str">
+        <v>O Sol é para Todos</v>
+      </c>
+      <c r="B268">
+        <v>1962</v>
+      </c>
+      <c r="C268" t="str">
+        <v>2h 9m</v>
+      </c>
+      <c r="D268">
+        <v>8.3</v>
+      </c>
+      <c r="E268" t="str">
+        <v>Atticus Finch, um advogado no sul da era da Depressão, defende um homem negro contra uma acusação de estupro imerecida, e seus filhos contra o preconceito.</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="str">
+        <v>Duro de Matar</v>
+      </c>
+      <c r="B269">
+        <v>1988</v>
+      </c>
+      <c r="C269" t="str">
+        <v>2h 12m</v>
+      </c>
+      <c r="D269">
+        <v>8.2</v>
+      </c>
+      <c r="E269" t="str">
+        <v>John McClane, agente do departamento de polícia de Nova York, tenta salvar sua esposa, Holly Gennaro, e outras pessoas que o terrorista alemão Hans Gruber tomou como reféns durante a festa de Natal no Nakatomi Plaza, em Los Angeles.</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="str">
+        <v>Golpe de Mestre</v>
+      </c>
+      <c r="B270">
+        <v>1973</v>
+      </c>
+      <c r="C270" t="str">
+        <v>2h 9m</v>
+      </c>
+      <c r="D270">
+        <v>8.2</v>
+      </c>
+      <c r="E270" t="str">
+        <v>Dois golpistas se reúnem para obter o melhor golpe.</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="str">
+        <v>Laranja Mecânica</v>
+      </c>
+      <c r="B271">
+        <v>1971</v>
+      </c>
+      <c r="C271" t="str">
+        <v>2h 16m</v>
+      </c>
+      <c r="D271">
+        <v>8.2</v>
+      </c>
+      <c r="E271" t="str">
+        <v>No futuro, um jovem líder de gang é levado para prisão e decide ser voluntário em um experimento, mas os resultados não são os esperados.</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="str">
+        <v>Snatch - Porcos e Diamantes</v>
+      </c>
+      <c r="B272">
+        <v>2000</v>
+      </c>
+      <c r="C272" t="str">
+        <v>1h 44m</v>
+      </c>
+      <c r="D272">
+        <v>8.2</v>
+      </c>
+      <c r="E272" t="str">
+        <v>Um ladrão amante dos jogos reúne gângsteres desprezíveis, um grupo de nômades irlandeses e uma fazenda de porcos em meio a chantagens, fraudes, boxeadores, um cão faminto e um grande diamante.</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="str">
+        <v>1917</v>
+      </c>
+      <c r="B273">
+        <v>2019</v>
+      </c>
+      <c r="C273" t="str">
+        <v>1h 59m</v>
+      </c>
+      <c r="D273">
+        <v>8.2</v>
+      </c>
+      <c r="E273" t="str">
+        <v>Na Primeira Guerra Mundial, dois soldados britânicos recebem ordens aparentemente impossíveis de cumprir. Em uma corrida contra o tempo, eles precisam atravessar o território inimigo e entregar uma mensagem que pode salvar 1.600 homens.</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="str">
+        <v>Los Angeles: Cidade Proibida</v>
+      </c>
+      <c r="B274">
+        <v>1997</v>
+      </c>
+      <c r="C274" t="str">
+        <v>2h 18m</v>
+      </c>
+      <c r="D274">
+        <v>8.2</v>
+      </c>
+      <c r="E274" t="str">
+        <v>A corrupção cresce em Los Angeles nos anos 50. Três policiais estão investigando uma série de assassinatos com sua própria marca de justiça.</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="str">
+        <v>A Queda! As Últimas Horas de Hitler</v>
+      </c>
+      <c r="B275">
+        <v>2004</v>
+      </c>
+      <c r="C275" t="str">
+        <v>2h 36m</v>
+      </c>
+      <c r="D275">
+        <v>8.2</v>
+      </c>
+      <c r="E275" t="str">
+        <v>O último secretário de Hitler relata seus últimos dias em seu bunker de Berlim no final da Segunda Guerra Mundial.</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="str">
+        <v>Ladrões de Bicicletas</v>
+      </c>
+      <c r="B276">
+        <v>1948</v>
+      </c>
+      <c r="C276" t="str">
+        <v>1h 29m</v>
+      </c>
+      <c r="D276">
+        <v>8.2</v>
+      </c>
+      <c r="E276" t="str">
+        <v>Na Itália da pós-guerra a bicicleta de um homem da classe trabalhadora é roubada. Ele e o filho partiram para encontrá-la.</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="str">
+        <v>Dangal</v>
+      </c>
+      <c r="B277">
+        <v>2016</v>
+      </c>
+      <c r="C277" t="str">
+        <v>2h 41m</v>
+      </c>
+      <c r="D277">
+        <v>8.3</v>
+      </c>
+      <c r="E277" t="str">
+        <v>O lutador Mahavir e suas filhas lutadoras procuram a gloria contra a opressão social nos jogos do Commonwealth.</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="str">
+        <v>Green Book: O Guia</v>
+      </c>
+      <c r="B278">
+        <v>2018</v>
+      </c>
+      <c r="C278" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D278">
+        <v>8.2</v>
+      </c>
+      <c r="E278" t="str">
+        <v>Um valentão ítalo-americano se torna o motorista de um pianista afro-americano em um tour no sul dos Estados Unidos nos anos sessenta.</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="str">
+        <v>O Show de Truman: O Show da Vida</v>
+      </c>
+      <c r="B279">
+        <v>1998</v>
+      </c>
+      <c r="C279" t="str">
+        <v>1h 43m</v>
+      </c>
+      <c r="D279">
+        <v>8.2</v>
+      </c>
+      <c r="E279" t="str">
+        <v>Um vendedor de seguros descobre que sua vida é um programa de televisão.</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="str">
+        <v>Hamilton</v>
+      </c>
+      <c r="B280">
+        <v>2020</v>
+      </c>
+      <c r="C280" t="str">
+        <v>2h 40m</v>
+      </c>
+      <c r="D280">
+        <v>8.3</v>
+      </c>
+      <c r="E280" t="str">
+        <v>A vida de um dos maiores fundadores e primeiro secretário do Tesouro da América, Alexander Hamilton.</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="str">
+        <v>Taxi Driver: Motorista de Táxi</v>
+      </c>
+      <c r="B281">
+        <v>1976</v>
+      </c>
+      <c r="C281" t="str">
+        <v>1h 54m</v>
+      </c>
+      <c r="D281">
+        <v>8.2</v>
+      </c>
+      <c r="E281" t="str">
+        <v>Um veterano de guerra mentalmente instável trabalha à noite como taxista na cidade de Nova York, onde a decadência e o desprezo alimentam seu desejo de ação violenta.</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="str">
+        <v>Batman Begins</v>
+      </c>
+      <c r="B282">
+        <v>2005</v>
+      </c>
+      <c r="C282" t="str">
+        <v>2h 20m</v>
+      </c>
+      <c r="D282">
+        <v>8.2</v>
+      </c>
+      <c r="E282" t="str">
+        <v>Após testemunhar a morte dos pais, o bilionário Bruce Wayne aprende a arte de lutar para confrontar a injustiça. Quando ele retorna a Gotham como Batman, ele deve deter uma sociedade secreta que pretende destruir a cidade.</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="str">
+        <v>Por uns Dólares a Mais</v>
+      </c>
+      <c r="B283">
+        <v>1965</v>
+      </c>
+      <c r="C283" t="str">
+        <v>2h 12m</v>
+      </c>
+      <c r="D283">
+        <v>8.2</v>
+      </c>
+      <c r="E283" t="str">
+        <v>Dois caçadores de recompensas com as mesmas intenções se reúnem para encontrar um criminoso ocidental.</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="str">
+        <v>Hababam Sinifi Sinifta Kaldi</v>
+      </c>
+      <c r="B284">
+        <v>1975</v>
+      </c>
+      <c r="C284" t="str">
+        <v>1h 35m</v>
+      </c>
+      <c r="D284">
+        <v>8.6</v>
+      </c>
+      <c r="E284" t="str">
+        <v>A young and beautiful female teacher starts working in an all boys high school.</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="str">
+        <v>Ilha do Medo</v>
+      </c>
+      <c r="B285">
+        <v>2010</v>
+      </c>
+      <c r="C285" t="str">
+        <v>2h 18m</v>
+      </c>
+      <c r="D285">
+        <v>8.2</v>
+      </c>
+      <c r="E285" t="str">
+        <v>Em 1954, um policial federal dos Estados Unidos investiga o desaparecimento de um assassino que escapou de um hospital psiquiátrico.</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="str">
+        <v>Meu Pai</v>
+      </c>
+      <c r="B286">
+        <v>2020</v>
+      </c>
+      <c r="C286" t="str">
+        <v>1h 37m</v>
+      </c>
+      <c r="D286">
+        <v>8.2</v>
+      </c>
+      <c r="E286" t="str">
+        <v>Um homem recusa toda a ajuda de sua filha à medida que envelhece. Enquanto ele tenta entender o que está acontecendo ao seu redor, ele começa a duvidar dos seus entes queridos, da sua mente e até mesmo da estrutura de sua realidade.</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="str">
+        <v>Sangue Negro</v>
+      </c>
+      <c r="B287">
+        <v>2007</v>
+      </c>
+      <c r="C287" t="str">
+        <v>2h 38m</v>
+      </c>
+      <c r="D287">
+        <v>8.2</v>
+      </c>
+      <c r="E287" t="str">
+        <v>Uma história sobre familia, religião, ódio e loucura, centrada na vida de um explorador de petróleo nos primeiros anos do negócio.</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="str">
+        <v>O Sexto Sentido</v>
+      </c>
+      <c r="B288">
+        <v>1999</v>
+      </c>
+      <c r="C288" t="str">
+        <v>1h 47m</v>
+      </c>
+      <c r="D288">
+        <v>8.2</v>
+      </c>
+      <c r="E288" t="str">
+        <v>Um menino que consegue se comunicar com espíritos encontra ajuda de um psicólogo.</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="str">
+        <v>Ran</v>
+      </c>
+      <c r="B289">
+        <v>1985</v>
+      </c>
+      <c r="C289" t="str">
+        <v>2h 40m</v>
+      </c>
+      <c r="D289">
+        <v>8.2</v>
+      </c>
+      <c r="E289" t="str">
+        <v>No Japão medieval, um senhor feudal decide abdicar e entregar seus domínios aos seus três filhos. Mas ele não é capaz de ver que esses novos poderes irão corrompê-los e levá-los a enfrentar um ao outro, e contra ele.</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="str">
+        <v>Cassino</v>
+      </c>
+      <c r="B290">
+        <v>1995</v>
+      </c>
+      <c r="C290" t="str">
+        <v>2h 58m</v>
+      </c>
+      <c r="D290">
+        <v>8.2</v>
+      </c>
+      <c r="E290" t="str">
+        <v>Uma história de ganância, dinheiro e assassinato acontece entre dois melhores amigos: um mafioso e um executivo de cassino, que competem uns com os outros por um império de jogo e pelo amor de uma socialite.</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="str">
+        <v>Onde os Fracos Não Têm Vez</v>
+      </c>
+      <c r="B291">
+        <v>2007</v>
+      </c>
+      <c r="C291" t="str">
+        <v>2h 2m</v>
+      </c>
+      <c r="D291">
+        <v>8.2</v>
+      </c>
+      <c r="E291" t="str">
+        <v>Violência e caos surgem quando um caçador se depara com uma negociação de drogas que deu errado e mais de dois milhões de dólares perto do Rio Grande.</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="str">
+        <v>Top Gun: Maverick</v>
+      </c>
+      <c r="B292">
+        <v>2022</v>
+      </c>
+      <c r="C292" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D292">
+        <v>8.2</v>
+      </c>
+      <c r="E292" t="str">
+        <v>Após mais de trinta anos de serviço como um dos melhores aviadores da Marinha, Pete Mitchell está onde pertence, ultrapassando os limites como um piloto de teste intrépido e evitando a promoção de posto que o manteria em terra.</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="str">
+        <v>O Enigma de Outro Mundo</v>
+      </c>
+      <c r="B293">
+        <v>1982</v>
+      </c>
+      <c r="C293" t="str">
+        <v>1h 49m</v>
+      </c>
+      <c r="D293">
+        <v>8.2</v>
+      </c>
+      <c r="E293" t="str">
+        <v>Uma equipe de pesquisa na Antártica é caçada por um alienígena que muda de forma e assume a aparência de suas vítimas.</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="str">
+        <v>Os Imperdoáveis</v>
+      </c>
+      <c r="B294">
+        <v>1992</v>
+      </c>
+      <c r="C294" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D294">
+        <v>8.2</v>
+      </c>
+      <c r="E294" t="str">
+        <v>O atirador do Velho Oeste, William Munny, relutantemente aceita um último trabalho com a ajuda de seu antigo amigo e um jovem.</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="str">
+        <v>O Labirinto do Fauno</v>
+      </c>
+      <c r="B295">
+        <v>2006</v>
+      </c>
+      <c r="C295" t="str">
+        <v>1h 58m</v>
+      </c>
+      <c r="D295">
+        <v>8.2</v>
+      </c>
+      <c r="E295" t="str">
+        <v>Na Espanha de 1944, a filha dum oficial do exército escapa a um mundo de fantasia.</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="str">
+        <v>Kill Bill: Volume 1</v>
+      </c>
+      <c r="B296">
+        <v>2003</v>
+      </c>
+      <c r="C296" t="str">
+        <v>1h 51m</v>
+      </c>
+      <c r="D296">
+        <v>8.2</v>
+      </c>
+      <c r="E296" t="str">
+        <v>Depois de despertar de um coma de quatro anos, uma antiga assassina busca vingança contra o grupo de assassinos que a traiu.</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="str">
+        <v>Os Suspeitos</v>
+      </c>
+      <c r="B297">
+        <v>2013</v>
+      </c>
+      <c r="C297" t="str">
+        <v>2h 33m</v>
+      </c>
+      <c r="D297">
+        <v>8.2</v>
+      </c>
+      <c r="E297" t="str">
+        <v>O único sobrevivente conta os torcidos eventos duma luta com pistolas num bote, quanfo cinco criminais eram levados pela polícia.</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="str">
+        <v>Uma Mente Brilhante</v>
+      </c>
+      <c r="B298">
+        <v>2001</v>
+      </c>
+      <c r="C298" t="str">
+        <v>2h 15m</v>
+      </c>
+      <c r="D298">
+        <v>8.2</v>
+      </c>
+      <c r="E298" t="str">
+        <v>A vida do brilhante mas insociável matemático John Nash muda quando ele aceita um trabalho secreto em criptografia.</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="str">
+        <v>O Melhor da Juventude</v>
+      </c>
+      <c r="B299">
+        <v>2003</v>
+      </c>
+      <c r="C299" t="str">
+        <v>6h 14m</v>
+      </c>
+      <c r="D299">
+        <v>8.4</v>
+      </c>
+      <c r="E299" t="str">
+        <v>Um épico italiano que segue a vida de dois irmãos, das décadas de 1960 a 2000.</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="str">
+        <v>Fugindo do Inferno</v>
+      </c>
+      <c r="B300">
+        <v>1963</v>
+      </c>
+      <c r="C300" t="str">
+        <v>2h 52m</v>
+      </c>
+      <c r="D300">
+        <v>8.2</v>
+      </c>
+      <c r="E300" t="str">
+        <v>Prisioneiros de guerra aliados planejam uma fuga maciça de um campo alemão durante a Segunda Guerra Mundial.</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="str">
+        <v>O Homem Elefante</v>
+      </c>
+      <c r="B301">
+        <v>1980</v>
+      </c>
+      <c r="C301" t="str">
+        <v>2h 4m</v>
+      </c>
+      <c r="D301">
+        <v>8.2</v>
+      </c>
+      <c r="E301" t="str">
+        <v>Um cirurgião vitoriano resgata um homem gravemente desfigurado que é maltratado enquanto tenta sobreviver como uma atração de circo. Por trás de sua aparência monstruosa, revela-se uma pessoa de bondade, inteligência e sofisticação.</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" t="str">
+        <v>Klaus</v>
+      </c>
+      <c r="B302">
+        <v>2019</v>
+      </c>
+      <c r="C302" t="str">
+        <v>1h 36m</v>
+      </c>
+      <c r="D302">
+        <v>8.2</v>
+      </c>
+      <c r="E302" t="str">
+        <v>Um simples ato de bondade sempre provoca outro, mesmo em um lugar gelado e distante. Quando o novo carteiro de Smeerensburg faz amizade com o fabricante de brinquedos Klaus, seus presentes derreteram uma antiga inimizade.</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="str">
+        <v>Disque M para Matar</v>
+      </c>
+      <c r="B303">
+        <v>1954</v>
+      </c>
+      <c r="C303" t="str">
+        <v>1h 45m</v>
+      </c>
+      <c r="D303">
+        <v>8.2</v>
+      </c>
+      <c r="E303" t="str">
+        <v>Um ex-tenista decide matar a esposa para herdar o dinheiro dela e se vingar de um caso que ela havia tido. A fim de se livrar de culpas, usa um antigo colega de faculdade. Mas as coisas não vão correr como estava planeado.</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="str">
+        <v>O Segredo dos Seus Olhos</v>
+      </c>
+      <c r="B304">
+        <v>2009</v>
+      </c>
+      <c r="C304" t="str">
+        <v>2h 9m</v>
+      </c>
+      <c r="D304">
+        <v>8.2</v>
+      </c>
+      <c r="E304" t="str">
+        <v>Um assessor jurídico aposentado escreve um romance com a esperança de fechar um de seus antigos casos de homicídio, que permanece sem solução, e superar o amor não correspondido que sentia por seu chefe. Décadas depois, ambas as memórias continuam a persegui-lo.</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="str">
+        <v>Chinatown</v>
+      </c>
+      <c r="B305">
+        <v>1974</v>
+      </c>
+      <c r="C305" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D305">
+        <v>8.1</v>
+      </c>
+      <c r="E305" t="str">
+        <v>Um detetive particular contratado para desmascarar um adúltero é pego em uma teia de fraude, corrupção e assassinato.</v>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="str">
+        <v>Jogos, Trapaças e Dois Canos Fumegantes</v>
+      </c>
+      <c r="B306">
+        <v>1998</v>
+      </c>
+      <c r="C306" t="str">
+        <v>1h 47m</v>
+      </c>
+      <c r="D306">
+        <v>8.1</v>
+      </c>
+      <c r="E306" t="str">
+        <v>Um jogo de cartas em Londres desencadeia um confronto entre quatro amigos, plantadores de maconha, agiotas e cobradores de dívidas em uma série de eventos curiosos, tudo por algo de maria, dinheiro e duas pistolas antigas.</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="str">
+        <v>V de Vingança</v>
+      </c>
+      <c r="B307">
+        <v>2005</v>
+      </c>
+      <c r="C307" t="str">
+        <v>2h 12m</v>
+      </c>
+      <c r="D307">
+        <v>8.1</v>
+      </c>
+      <c r="E307" t="str">
+        <v>Em um futuro da tirania britânica, um lutador clandestino conhecido como V trama um plano para derrubá-la com a ajuda de uma jovem mulher.</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="str">
+        <v>Rashomon</v>
+      </c>
+      <c r="B308">
+        <v>1950</v>
+      </c>
+      <c r="C308" t="str">
+        <v>1h 28m</v>
+      </c>
+      <c r="D308">
+        <v>8.1</v>
+      </c>
+      <c r="E308" t="str">
+        <v>A violação de uma noiva e o assassinato de seu marido samurai são lembrados desde a perspectiva de um bandido, da noiva, do fantasma do samurai e de um lenhador.</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="str">
+        <v>Três Anúncios para um Crime</v>
+      </c>
+      <c r="B309">
+        <v>2017</v>
+      </c>
+      <c r="C309" t="str">
+        <v>1h 55m</v>
+      </c>
+      <c r="D309">
+        <v>8.1</v>
+      </c>
+      <c r="E309" t="str">
+        <v>Uma mãe desafia pessoalmente as autoridades locais para resolver o assassinato de sua filha.</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="str">
+        <v>Prenda-Me se for Capaz</v>
+      </c>
+      <c r="B310">
+        <v>2002</v>
+      </c>
+      <c r="C310" t="str">
+        <v>2h 21m</v>
+      </c>
+      <c r="D310">
+        <v>8.1</v>
+      </c>
+      <c r="E310" t="str">
+        <v>Um agente do FBI persegue Frank Abagnale, que antes de seus 19 anos consegue ganhar milhões de dólares fingindo ser um piloto, um médico e um advogado.</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="str">
+        <v>Trainspotting: Sem Limites</v>
+      </c>
+      <c r="B311">
+        <v>1996</v>
+      </c>
+      <c r="C311" t="str">
+        <v>1h 33m</v>
+      </c>
+      <c r="D311">
+        <v>8.1</v>
+      </c>
+      <c r="E311" t="str">
+        <v>Renton, profundamente imerso no mundo das drogas em Edimburgo, tenta sair do ambiente apesar da má influência dos amigos.</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="str">
+        <v>A Ponte do Rio Kwai</v>
+      </c>
+      <c r="B312">
+        <v>1957</v>
+      </c>
+      <c r="C312" t="str">
+        <v>2h 41m</v>
+      </c>
+      <c r="D312">
+        <v>8.1</v>
+      </c>
+      <c r="E312" t="str">
+        <v>Depois de resolver suas diferenças com um japonês, o comandante do campo, um coronel britânico, coopera para supervisionar a construção de uma ponte ferroviária.</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="str">
+        <v>Touro Indomável</v>
+      </c>
+      <c r="B313">
+        <v>1980</v>
+      </c>
+      <c r="C313" t="str">
+        <v>2h 9m</v>
+      </c>
+      <c r="D313">
+        <v>8.1</v>
+      </c>
+      <c r="E313" t="str">
+        <v>A vida do boxeador Jake LaMotta, cuja violência e temperamento que o levaram até o topo dos ringues destruíram a sua vida fora deles.</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="str">
+        <v>Harry Potter e as Relíquias da Morte - Parte 2</v>
+      </c>
+      <c r="B314">
+        <v>2011</v>
+      </c>
+      <c r="C314" t="str">
+        <v>2h 10m</v>
+      </c>
+      <c r="D314">
+        <v>8.1</v>
+      </c>
+      <c r="E314" t="str">
+        <v>Conforme a batalha entre as forças do bem e do mal no mundo bruxo aumenta de proporções, Harry Potter se aproxima cada vez mais do confronto final com Voldemort.</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="str">
+        <v>Fargo: Uma Comédia de Erros</v>
+      </c>
+      <c r="B315">
+        <v>1996</v>
+      </c>
+      <c r="C315" t="str">
+        <v>1h 38m</v>
+      </c>
+      <c r="D315">
+        <v>8.1</v>
+      </c>
+      <c r="E315" t="str">
+        <v>O crime de Jerry Lundegaard se desfaz devido à falta de sorte dele e de seus colegas e ao persistente trabalho polícia.</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="str">
+        <v>Guerreiro</v>
+      </c>
+      <c r="B316">
+        <v>2011</v>
+      </c>
+      <c r="C316" t="str">
+        <v>2h 20m</v>
+      </c>
+      <c r="D316">
+        <v>8.1</v>
+      </c>
+      <c r="E316" t="str">
+        <v>O filho pequeno de um exboxer alcoólatra volta para casa, onde seu pai o treina para um torneio de artes marciais mistas.</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="str">
+        <v>Sociedade dos Poetas Mortos</v>
+      </c>
+      <c r="B317">
+        <v>1989</v>
+      </c>
+      <c r="C317" t="str">
+        <v>2h 8m</v>
+      </c>
+      <c r="D317">
+        <v>8.1</v>
+      </c>
+      <c r="E317" t="str">
+        <v>O professor de Inglés John Keating inspira a seus estudantes a ver a poesia duma perspectiva diferente.</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="str">
+        <v>Menina de Ouro</v>
+      </c>
+      <c r="B318">
+        <v>2004</v>
+      </c>
+      <c r="C318" t="str">
+        <v>2h 12m</v>
+      </c>
+      <c r="D318">
+        <v>8.1</v>
+      </c>
+      <c r="E318" t="str">
+        <v>Uma mulher determinada se prepara para se tornar numa pugilista profissional.</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="str">
+        <v>Ben-Hur</v>
+      </c>
+      <c r="B319">
+        <v>1959</v>
+      </c>
+      <c r="C319" t="str">
+        <v>3h 32m</v>
+      </c>
+      <c r="D319">
+        <v>8.1</v>
+      </c>
+      <c r="E319" t="str">
+        <v>Quando um príncipe de Jerusalém é traído e enviado à escravidão por um amigo romano, ele recupera sua liberdade e retorna para se vingar.</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="str">
+        <v>Gran Torino</v>
+      </c>
+      <c r="B320">
+        <v>2008</v>
+      </c>
+      <c r="C320" t="str">
+        <v>1h 56m</v>
+      </c>
+      <c r="D320">
+        <v>8.1</v>
+      </c>
+      <c r="E320" t="str">
+        <v>Walt Kowalski, um ranzinza veterano da guerra da Coreia, tenta dar uma lição em seu vizinho quando este tentar roubar seu bem mais precioso: um Gran Torino de 1972.</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="str">
+        <v>Demon Slayer: Kimetsu no Yaiba - Castelo Infinito</v>
+      </c>
+      <c r="B321">
+        <v>2025</v>
+      </c>
+      <c r="C321" t="str">
+        <v>2h 35m</v>
+      </c>
+      <c r="D321">
+        <v>8.6</v>
+      </c>
+      <c r="E321" t="str">
+        <v>O Corpo de Caçadores de Demônios mergulha no Castelo do Infinito para derrotar Muzan.</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E191"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E321"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>